<commit_message>
GSCHED-838: Update telescope scheduler
</commit_message>
<xml_diff>
--- a/scheduler/services/resource/data/simulation/telescope_schedules.xlsx
+++ b/scheduler/services/resource/data/simulation/telescope_schedules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmiller/python/scheduler/scheduler/services/resource/data/simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmiller/gemini/sciops/softdevel/Queue_planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C89321-DE9D-484E-90DF-A4144F740B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DE8010-A9BE-3444-A135-8DBFD9ACCCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36340" yWindow="500" windowWidth="36000" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21600" yWindow="500" windowWidth="36000" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12548" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13633" uniqueCount="39">
   <si>
     <t>Local Date</t>
   </si>
@@ -145,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -158,12 +158,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -223,7 +225,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -443,13 +445,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD366"/>
+  <dimension ref="A1:AD397"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B332" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B343" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A366"/>
+      <selection pane="bottomRight" activeCell="C385" sqref="C385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23380,6 +23382,2176 @@
       <c r="AC366" s="2"/>
       <c r="AD366" s="2"/>
     </row>
+    <row r="367" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A367" s="5">
+        <v>45870</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E367" s="2"/>
+      <c r="F367" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G367" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H367" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I367" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J367" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L367" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N367" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O367" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U367" s="2"/>
+      <c r="V367" s="2"/>
+      <c r="W367" s="2"/>
+      <c r="X367" s="2"/>
+      <c r="Y367" s="2"/>
+      <c r="Z367" s="2"/>
+      <c r="AA367" s="2"/>
+      <c r="AB367" s="2"/>
+      <c r="AC367" s="2"/>
+      <c r="AD367" s="2"/>
+    </row>
+    <row r="368" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A368" s="5">
+        <v>45871</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E368" s="2"/>
+      <c r="F368" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H368" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I368" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J368" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L368" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N368" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O368" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U368" s="2"/>
+      <c r="V368" s="2"/>
+      <c r="W368" s="2"/>
+      <c r="X368" s="2"/>
+      <c r="Y368" s="2"/>
+      <c r="Z368" s="2"/>
+      <c r="AA368" s="2"/>
+      <c r="AB368" s="2"/>
+      <c r="AC368" s="2"/>
+      <c r="AD368" s="2"/>
+    </row>
+    <row r="369" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A369" s="5">
+        <v>45872</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E369" s="2"/>
+      <c r="F369" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H369" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I369" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J369" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L369" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N369" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O369" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U369" s="2"/>
+      <c r="V369" s="2"/>
+      <c r="W369" s="2"/>
+      <c r="X369" s="2"/>
+      <c r="Y369" s="2"/>
+      <c r="Z369" s="2"/>
+      <c r="AA369" s="2"/>
+      <c r="AB369" s="2"/>
+      <c r="AC369" s="2"/>
+      <c r="AD369" s="2"/>
+    </row>
+    <row r="370" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A370" s="5">
+        <v>45873</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E370" s="2"/>
+      <c r="F370" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H370" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I370" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J370" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L370" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N370" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O370" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U370" s="2"/>
+      <c r="V370" s="2"/>
+      <c r="W370" s="2"/>
+      <c r="X370" s="2"/>
+      <c r="Y370" s="2"/>
+      <c r="Z370" s="2"/>
+      <c r="AA370" s="2"/>
+      <c r="AB370" s="2"/>
+      <c r="AC370" s="2"/>
+      <c r="AD370" s="2"/>
+    </row>
+    <row r="371" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A371" s="5">
+        <v>45874</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E371" s="2"/>
+      <c r="F371" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G371" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H371" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I371" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J371" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L371" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N371" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O371" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U371" s="2"/>
+      <c r="V371" s="2"/>
+      <c r="W371" s="2"/>
+      <c r="X371" s="2"/>
+      <c r="Y371" s="2"/>
+      <c r="Z371" s="2"/>
+      <c r="AA371" s="2"/>
+      <c r="AB371" s="2"/>
+      <c r="AC371" s="2"/>
+      <c r="AD371" s="2"/>
+    </row>
+    <row r="372" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A372" s="5">
+        <v>45875</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E372" s="2"/>
+      <c r="F372" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G372" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H372" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I372" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J372" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L372" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N372" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O372" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U372" s="2"/>
+      <c r="V372" s="2"/>
+      <c r="W372" s="2"/>
+      <c r="X372" s="2"/>
+      <c r="Y372" s="2"/>
+      <c r="Z372" s="2"/>
+      <c r="AA372" s="2"/>
+      <c r="AB372" s="2"/>
+      <c r="AC372" s="2"/>
+      <c r="AD372" s="2"/>
+    </row>
+    <row r="373" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A373" s="5">
+        <v>45876</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E373" s="2"/>
+      <c r="F373" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G373" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H373" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I373" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J373" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L373" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N373" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O373" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U373" s="2"/>
+      <c r="V373" s="2"/>
+      <c r="W373" s="2"/>
+      <c r="X373" s="2"/>
+      <c r="Y373" s="2"/>
+      <c r="Z373" s="2"/>
+      <c r="AA373" s="2"/>
+      <c r="AB373" s="2"/>
+      <c r="AC373" s="2"/>
+      <c r="AD373" s="2"/>
+    </row>
+    <row r="374" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A374" s="5">
+        <v>45877</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E374" s="2"/>
+      <c r="F374" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G374" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H374" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I374" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J374" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L374" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N374" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O374" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U374" s="2"/>
+      <c r="V374" s="2"/>
+      <c r="W374" s="2"/>
+      <c r="X374" s="2"/>
+      <c r="Y374" s="2"/>
+      <c r="Z374" s="2"/>
+      <c r="AA374" s="2"/>
+      <c r="AB374" s="2"/>
+      <c r="AC374" s="2"/>
+      <c r="AD374" s="2"/>
+    </row>
+    <row r="375" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A375" s="5">
+        <v>45878</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E375" s="2"/>
+      <c r="F375" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G375" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H375" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I375" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J375" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L375" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N375" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O375" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U375" s="2"/>
+      <c r="V375" s="2"/>
+      <c r="W375" s="2"/>
+      <c r="X375" s="2"/>
+      <c r="Y375" s="2"/>
+      <c r="Z375" s="2"/>
+      <c r="AA375" s="2"/>
+      <c r="AB375" s="2"/>
+      <c r="AC375" s="2"/>
+      <c r="AD375" s="2"/>
+    </row>
+    <row r="376" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A376" s="5">
+        <v>45879</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E376" s="2"/>
+      <c r="F376" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G376" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H376" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I376" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J376" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L376" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N376" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O376" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U376" s="2"/>
+      <c r="V376" s="2"/>
+      <c r="W376" s="2"/>
+      <c r="X376" s="2"/>
+      <c r="Y376" s="2"/>
+      <c r="Z376" s="2"/>
+      <c r="AA376" s="2"/>
+      <c r="AB376" s="2"/>
+      <c r="AC376" s="2"/>
+      <c r="AD376" s="2"/>
+    </row>
+    <row r="377" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A377" s="5">
+        <v>45880</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E377" s="2"/>
+      <c r="F377" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G377" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H377" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I377" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J377" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L377" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N377" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O377" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U377" s="2"/>
+      <c r="V377" s="2"/>
+      <c r="W377" s="2"/>
+      <c r="X377" s="2"/>
+      <c r="Y377" s="2"/>
+      <c r="Z377" s="2"/>
+      <c r="AA377" s="2"/>
+      <c r="AB377" s="2"/>
+      <c r="AC377" s="2"/>
+      <c r="AD377" s="2"/>
+    </row>
+    <row r="378" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A378" s="5">
+        <v>45881</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E378" s="2"/>
+      <c r="F378" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G378" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H378" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I378" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J378" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L378" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N378" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O378" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U378" s="2"/>
+      <c r="V378" s="2"/>
+      <c r="W378" s="2"/>
+      <c r="X378" s="2"/>
+      <c r="Y378" s="2"/>
+      <c r="Z378" s="2"/>
+      <c r="AA378" s="2"/>
+      <c r="AB378" s="2"/>
+      <c r="AC378" s="2"/>
+      <c r="AD378" s="2"/>
+    </row>
+    <row r="379" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A379" s="5">
+        <v>45882</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E379" s="2"/>
+      <c r="F379" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G379" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H379" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I379" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J379" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L379" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N379" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O379" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U379" s="2"/>
+      <c r="V379" s="2"/>
+      <c r="W379" s="2"/>
+      <c r="X379" s="2"/>
+      <c r="Y379" s="2"/>
+      <c r="Z379" s="2"/>
+      <c r="AA379" s="2"/>
+      <c r="AB379" s="2"/>
+      <c r="AC379" s="2"/>
+      <c r="AD379" s="2"/>
+    </row>
+    <row r="380" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A380" s="5">
+        <v>45883</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E380" s="2"/>
+      <c r="F380" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G380" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H380" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I380" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J380" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L380" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N380" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O380" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U380" s="2"/>
+      <c r="V380" s="2"/>
+      <c r="W380" s="2"/>
+      <c r="X380" s="2"/>
+      <c r="Y380" s="2"/>
+      <c r="Z380" s="2"/>
+      <c r="AA380" s="2"/>
+      <c r="AB380" s="2"/>
+      <c r="AC380" s="2"/>
+      <c r="AD380" s="2"/>
+    </row>
+    <row r="381" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A381" s="5">
+        <v>45884</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E381" s="2"/>
+      <c r="F381" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G381" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H381" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I381" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J381" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L381" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N381" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O381" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U381" s="2"/>
+      <c r="V381" s="2"/>
+      <c r="W381" s="2"/>
+      <c r="X381" s="2"/>
+      <c r="Y381" s="2"/>
+      <c r="Z381" s="2"/>
+      <c r="AA381" s="2"/>
+      <c r="AB381" s="2"/>
+      <c r="AC381" s="2"/>
+      <c r="AD381" s="2"/>
+    </row>
+    <row r="382" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A382" s="5">
+        <v>45885</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E382" s="2"/>
+      <c r="F382" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G382" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H382" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I382" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J382" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L382" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N382" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O382" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U382" s="2"/>
+      <c r="V382" s="2"/>
+      <c r="W382" s="2"/>
+      <c r="X382" s="2"/>
+      <c r="Y382" s="2"/>
+      <c r="Z382" s="2"/>
+      <c r="AA382" s="2"/>
+      <c r="AB382" s="2"/>
+      <c r="AC382" s="2"/>
+      <c r="AD382" s="2"/>
+    </row>
+    <row r="383" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A383" s="5">
+        <v>45886</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E383" s="2"/>
+      <c r="F383" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G383" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H383" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I383" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J383" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L383" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N383" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O383" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U383" s="2"/>
+      <c r="V383" s="2"/>
+      <c r="W383" s="2"/>
+      <c r="X383" s="2"/>
+      <c r="Y383" s="2"/>
+      <c r="Z383" s="2"/>
+      <c r="AA383" s="2"/>
+      <c r="AB383" s="2"/>
+      <c r="AC383" s="2"/>
+      <c r="AD383" s="2"/>
+    </row>
+    <row r="384" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A384" s="5">
+        <v>45887</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D384" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E384" s="2"/>
+      <c r="F384" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G384" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H384" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I384" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J384" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L384" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N384" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O384" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U384" s="2"/>
+      <c r="V384" s="2"/>
+      <c r="W384" s="2"/>
+      <c r="X384" s="2"/>
+      <c r="Y384" s="2"/>
+      <c r="Z384" s="2"/>
+      <c r="AA384" s="2"/>
+      <c r="AB384" s="2"/>
+      <c r="AC384" s="2"/>
+      <c r="AD384" s="2"/>
+    </row>
+    <row r="385" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A385" s="5">
+        <v>45888</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D385" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E385" s="2"/>
+      <c r="F385" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G385" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H385" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I385" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J385" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L385" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N385" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O385" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U385" s="2"/>
+      <c r="V385" s="2"/>
+      <c r="W385" s="2"/>
+      <c r="X385" s="2"/>
+      <c r="Y385" s="2"/>
+      <c r="Z385" s="2"/>
+      <c r="AA385" s="2"/>
+      <c r="AB385" s="2"/>
+      <c r="AC385" s="2"/>
+      <c r="AD385" s="2"/>
+    </row>
+    <row r="386" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A386" s="5">
+        <v>45889</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D386" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E386" s="2"/>
+      <c r="F386" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G386" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H386" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I386" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J386" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L386" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N386" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O386" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U386" s="2"/>
+      <c r="V386" s="2"/>
+      <c r="W386" s="2"/>
+      <c r="X386" s="2"/>
+      <c r="Y386" s="2"/>
+      <c r="Z386" s="2"/>
+      <c r="AA386" s="2"/>
+      <c r="AB386" s="2"/>
+      <c r="AC386" s="2"/>
+      <c r="AD386" s="2"/>
+    </row>
+    <row r="387" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A387" s="5">
+        <v>45890</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D387" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E387" s="2"/>
+      <c r="F387" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G387" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H387" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I387" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J387" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L387" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N387" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O387" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U387" s="2"/>
+      <c r="V387" s="2"/>
+      <c r="W387" s="2"/>
+      <c r="X387" s="2"/>
+      <c r="Y387" s="2"/>
+      <c r="Z387" s="2"/>
+      <c r="AA387" s="2"/>
+      <c r="AB387" s="2"/>
+      <c r="AC387" s="2"/>
+      <c r="AD387" s="2"/>
+    </row>
+    <row r="388" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A388" s="5">
+        <v>45891</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D388" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E388" s="2"/>
+      <c r="F388" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G388" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H388" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I388" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J388" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L388" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N388" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O388" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U388" s="2"/>
+      <c r="V388" s="2"/>
+      <c r="W388" s="2"/>
+      <c r="X388" s="2"/>
+      <c r="Y388" s="2"/>
+      <c r="Z388" s="2"/>
+      <c r="AA388" s="2"/>
+      <c r="AB388" s="2"/>
+      <c r="AC388" s="2"/>
+      <c r="AD388" s="2"/>
+    </row>
+    <row r="389" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A389" s="5">
+        <v>45892</v>
+      </c>
+      <c r="B389" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D389" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E389" s="2"/>
+      <c r="F389" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G389" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H389" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I389" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J389" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L389" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N389" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O389" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U389" s="2"/>
+      <c r="V389" s="2"/>
+      <c r="W389" s="2"/>
+      <c r="X389" s="2"/>
+      <c r="Y389" s="2"/>
+      <c r="Z389" s="2"/>
+      <c r="AA389" s="2"/>
+      <c r="AB389" s="2"/>
+      <c r="AC389" s="2"/>
+      <c r="AD389" s="2"/>
+    </row>
+    <row r="390" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A390" s="5">
+        <v>45893</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D390" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E390" s="2"/>
+      <c r="F390" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G390" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H390" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I390" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J390" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L390" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N390" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O390" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U390" s="2"/>
+      <c r="V390" s="2"/>
+      <c r="W390" s="2"/>
+      <c r="X390" s="2"/>
+      <c r="Y390" s="2"/>
+      <c r="Z390" s="2"/>
+      <c r="AA390" s="2"/>
+      <c r="AB390" s="2"/>
+      <c r="AC390" s="2"/>
+      <c r="AD390" s="2"/>
+    </row>
+    <row r="391" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A391" s="5">
+        <v>45894</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E391" s="2"/>
+      <c r="F391" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G391" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H391" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I391" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J391" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L391" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N391" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O391" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U391" s="2"/>
+      <c r="V391" s="2"/>
+      <c r="W391" s="2"/>
+      <c r="X391" s="2"/>
+      <c r="Y391" s="2"/>
+      <c r="Z391" s="2"/>
+      <c r="AA391" s="2"/>
+      <c r="AB391" s="2"/>
+      <c r="AC391" s="2"/>
+      <c r="AD391" s="2"/>
+    </row>
+    <row r="392" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A392" s="5">
+        <v>45895</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E392" s="2"/>
+      <c r="F392" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G392" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H392" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I392" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J392" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L392" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N392" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O392" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U392" s="2"/>
+      <c r="V392" s="2"/>
+      <c r="W392" s="2"/>
+      <c r="X392" s="2"/>
+      <c r="Y392" s="2"/>
+      <c r="Z392" s="2"/>
+      <c r="AA392" s="2"/>
+      <c r="AB392" s="2"/>
+      <c r="AC392" s="2"/>
+      <c r="AD392" s="2"/>
+    </row>
+    <row r="393" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A393" s="5">
+        <v>45896</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E393" s="2"/>
+      <c r="F393" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G393" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H393" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I393" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J393" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L393" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N393" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O393" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U393" s="2"/>
+      <c r="V393" s="2"/>
+      <c r="W393" s="2"/>
+      <c r="X393" s="2"/>
+      <c r="Y393" s="2"/>
+      <c r="Z393" s="2"/>
+      <c r="AA393" s="2"/>
+      <c r="AB393" s="2"/>
+      <c r="AC393" s="2"/>
+      <c r="AD393" s="2"/>
+    </row>
+    <row r="394" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A394" s="5">
+        <v>45897</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D394" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E394" s="2"/>
+      <c r="F394" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G394" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H394" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I394" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J394" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L394" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N394" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O394" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U394" s="2"/>
+      <c r="V394" s="2"/>
+      <c r="W394" s="2"/>
+      <c r="X394" s="2"/>
+      <c r="Y394" s="2"/>
+      <c r="Z394" s="2"/>
+      <c r="AA394" s="2"/>
+      <c r="AB394" s="2"/>
+      <c r="AC394" s="2"/>
+      <c r="AD394" s="2"/>
+    </row>
+    <row r="395" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A395" s="5">
+        <v>45898</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E395" s="2"/>
+      <c r="F395" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G395" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H395" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I395" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J395" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L395" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N395" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O395" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U395" s="2"/>
+      <c r="V395" s="2"/>
+      <c r="W395" s="2"/>
+      <c r="X395" s="2"/>
+      <c r="Y395" s="2"/>
+      <c r="Z395" s="2"/>
+      <c r="AA395" s="2"/>
+      <c r="AB395" s="2"/>
+      <c r="AC395" s="2"/>
+      <c r="AD395" s="2"/>
+    </row>
+    <row r="396" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A396" s="5">
+        <v>45899</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E396" s="2"/>
+      <c r="F396" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G396" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H396" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I396" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J396" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L396" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N396" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O396" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U396" s="2"/>
+      <c r="V396" s="2"/>
+      <c r="W396" s="2"/>
+      <c r="X396" s="2"/>
+      <c r="Y396" s="2"/>
+      <c r="Z396" s="2"/>
+      <c r="AA396" s="2"/>
+      <c r="AB396" s="2"/>
+      <c r="AC396" s="2"/>
+      <c r="AD396" s="2"/>
+    </row>
+    <row r="397" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A397" s="5">
+        <v>45900</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E397" s="2"/>
+      <c r="F397" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G397" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H397" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I397" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J397" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L397" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N397" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O397" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U397" s="2"/>
+      <c r="V397" s="2"/>
+      <c r="W397" s="2"/>
+      <c r="X397" s="2"/>
+      <c r="Y397" s="2"/>
+      <c r="Z397" s="2"/>
+      <c r="AA397" s="2"/>
+      <c r="AB397" s="2"/>
+      <c r="AC397" s="2"/>
+      <c r="AD397" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23391,13 +25563,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S366"/>
+  <dimension ref="A1:S397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B345" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L48" sqref="L48:L56"/>
+      <selection pane="bottomRight" activeCell="A386" sqref="A386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -43987,6 +46159,1773 @@
         <v>24</v>
       </c>
     </row>
+    <row r="367" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A367" s="5">
+        <v>45870</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D367" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E367" s="1"/>
+      <c r="F367" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G367" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H367" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I367" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J367" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M367" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N367" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O367" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S367" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="368" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A368" s="5">
+        <v>45871</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D368" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E368" s="1"/>
+      <c r="F368" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G368" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H368" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I368" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J368" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M368" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N368" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O368" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S368" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="369" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A369" s="5">
+        <v>45872</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D369" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E369" s="1"/>
+      <c r="F369" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G369" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H369" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I369" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J369" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M369" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N369" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O369" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S369" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="370" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A370" s="5">
+        <v>45873</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D370" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E370" s="1"/>
+      <c r="F370" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G370" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H370" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I370" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J370" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M370" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N370" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O370" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S370" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="371" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A371" s="5">
+        <v>45874</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D371" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E371" s="1"/>
+      <c r="F371" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I371" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J371" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M371" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N371" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O371" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S371" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="372" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A372" s="5">
+        <v>45875</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D372" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E372" s="1"/>
+      <c r="F372" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G372" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H372" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I372" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J372" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M372" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N372" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O372" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S372" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="373" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A373" s="5">
+        <v>45876</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D373" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E373" s="1"/>
+      <c r="F373" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G373" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H373" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I373" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J373" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M373" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N373" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O373" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S373" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="374" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A374" s="5">
+        <v>45877</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D374" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E374" s="1"/>
+      <c r="F374" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H374" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I374" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J374" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M374" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N374" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O374" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S374" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="375" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A375" s="5">
+        <v>45878</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D375" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E375" s="1"/>
+      <c r="F375" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G375" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I375" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J375" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M375" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N375" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O375" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S375" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="376" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A376" s="5">
+        <v>45879</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D376" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E376" s="1"/>
+      <c r="F376" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G376" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H376" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I376" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J376" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M376" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N376" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O376" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S376" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="377" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A377" s="5">
+        <v>45880</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D377" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E377" s="1"/>
+      <c r="F377" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H377" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I377" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J377" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M377" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N377" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O377" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S377" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="378" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A378" s="5">
+        <v>45881</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D378" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E378" s="1"/>
+      <c r="F378" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I378" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J378" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M378" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N378" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O378" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S378" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="379" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A379" s="5">
+        <v>45882</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D379" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E379" s="1"/>
+      <c r="F379" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G379" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H379" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I379" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J379" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M379" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N379" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O379" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S379" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="380" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A380" s="5">
+        <v>45883</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D380" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E380" s="1"/>
+      <c r="F380" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I380" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J380" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M380" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N380" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O380" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S380" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="381" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A381" s="5">
+        <v>45884</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D381" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E381" s="1"/>
+      <c r="F381" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G381" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H381" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I381" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J381" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M381" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N381" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O381" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S381" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="382" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A382" s="5">
+        <v>45885</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D382" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E382" s="1"/>
+      <c r="F382" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I382" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J382" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M382" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N382" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O382" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S382" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="383" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A383" s="5">
+        <v>45886</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D383" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E383" s="1"/>
+      <c r="F383" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G383" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H383" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I383" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J383" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M383" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N383" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O383" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S383" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="384" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A384" s="5">
+        <v>45887</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D384" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E384" s="1"/>
+      <c r="F384" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G384" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H384" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I384" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J384" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M384" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N384" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O384" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S384" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="385" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A385" s="5">
+        <v>45888</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D385" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E385" s="1"/>
+      <c r="F385" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G385" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H385" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I385" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J385" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M385" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N385" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O385" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S385" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="386" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A386" s="5">
+        <v>45889</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D386" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E386" s="1"/>
+      <c r="F386" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H386" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I386" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J386" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M386" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N386" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O386" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S386" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="387" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A387" s="5">
+        <v>45890</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D387" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E387" s="1"/>
+      <c r="F387" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G387" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H387" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I387" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J387" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M387" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N387" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O387" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S387" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="388" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A388" s="5">
+        <v>45891</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D388" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E388" s="1"/>
+      <c r="F388" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G388" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H388" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I388" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J388" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M388" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N388" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O388" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S388" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="389" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A389" s="5">
+        <v>45892</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D389" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E389" s="1"/>
+      <c r="F389" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H389" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I389" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J389" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M389" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N389" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O389" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S389" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="390" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A390" s="5">
+        <v>45893</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D390" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E390" s="1"/>
+      <c r="F390" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G390" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H390" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I390" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J390" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M390" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N390" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O390" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S390" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="391" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A391" s="5">
+        <v>45894</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D391" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E391" s="1"/>
+      <c r="F391" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H391" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I391" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J391" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M391" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N391" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O391" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S391" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="392" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A392" s="5">
+        <v>45895</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D392" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E392" s="1"/>
+      <c r="F392" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G392" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H392" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I392" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J392" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M392" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N392" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O392" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S392" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="393" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A393" s="5">
+        <v>45896</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D393" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E393" s="1"/>
+      <c r="F393" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H393" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I393" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J393" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M393" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N393" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O393" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S393" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="394" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A394" s="5">
+        <v>45897</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D394" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E394" s="1"/>
+      <c r="F394" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I394" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J394" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M394" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N394" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O394" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S394" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="395" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A395" s="5">
+        <v>45898</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D395" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E395" s="1"/>
+      <c r="F395" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G395" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H395" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I395" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J395" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M395" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N395" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O395" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S395" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="396" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A396" s="5">
+        <v>45899</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D396" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E396" s="1"/>
+      <c r="F396" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H396" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I396" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J396" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M396" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N396" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O396" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S396" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="397" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A397" s="5">
+        <v>45900</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D397" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E397" s="1"/>
+      <c r="F397" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G397" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H397" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I397" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J397" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M397" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N397" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O397" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S397" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GSCHED-838: Update Sim Services (#580)
* GSCHED-838: Modify builder to work with SimResource and add ToO data

* GSCHED-838: Modify sim resources to work with current ODB

* GSCHED-838: Update telescope scheduler

* GSCHED-838: Revert to default config
</commit_message>
<xml_diff>
--- a/scheduler/services/resource/data/simulation/telescope_schedules.xlsx
+++ b/scheduler/services/resource/data/simulation/telescope_schedules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmiller/python/scheduler/scheduler/services/resource/data/simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmiller/gemini/sciops/softdevel/Queue_planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C89321-DE9D-484E-90DF-A4144F740B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DE8010-A9BE-3444-A135-8DBFD9ACCCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36340" yWindow="500" windowWidth="36000" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21600" yWindow="500" windowWidth="36000" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12548" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13633" uniqueCount="39">
   <si>
     <t>Local Date</t>
   </si>
@@ -145,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -158,12 +158,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -223,7 +225,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -443,13 +445,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD366"/>
+  <dimension ref="A1:AD397"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B332" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B343" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A366"/>
+      <selection pane="bottomRight" activeCell="C385" sqref="C385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23380,6 +23382,2176 @@
       <c r="AC366" s="2"/>
       <c r="AD366" s="2"/>
     </row>
+    <row r="367" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A367" s="5">
+        <v>45870</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E367" s="2"/>
+      <c r="F367" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G367" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H367" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I367" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J367" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L367" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N367" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O367" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T367" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U367" s="2"/>
+      <c r="V367" s="2"/>
+      <c r="W367" s="2"/>
+      <c r="X367" s="2"/>
+      <c r="Y367" s="2"/>
+      <c r="Z367" s="2"/>
+      <c r="AA367" s="2"/>
+      <c r="AB367" s="2"/>
+      <c r="AC367" s="2"/>
+      <c r="AD367" s="2"/>
+    </row>
+    <row r="368" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A368" s="5">
+        <v>45871</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E368" s="2"/>
+      <c r="F368" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H368" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I368" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J368" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L368" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N368" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O368" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T368" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U368" s="2"/>
+      <c r="V368" s="2"/>
+      <c r="W368" s="2"/>
+      <c r="X368" s="2"/>
+      <c r="Y368" s="2"/>
+      <c r="Z368" s="2"/>
+      <c r="AA368" s="2"/>
+      <c r="AB368" s="2"/>
+      <c r="AC368" s="2"/>
+      <c r="AD368" s="2"/>
+    </row>
+    <row r="369" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A369" s="5">
+        <v>45872</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E369" s="2"/>
+      <c r="F369" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H369" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I369" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J369" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L369" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N369" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O369" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T369" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U369" s="2"/>
+      <c r="V369" s="2"/>
+      <c r="W369" s="2"/>
+      <c r="X369" s="2"/>
+      <c r="Y369" s="2"/>
+      <c r="Z369" s="2"/>
+      <c r="AA369" s="2"/>
+      <c r="AB369" s="2"/>
+      <c r="AC369" s="2"/>
+      <c r="AD369" s="2"/>
+    </row>
+    <row r="370" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A370" s="5">
+        <v>45873</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E370" s="2"/>
+      <c r="F370" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H370" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I370" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J370" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L370" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N370" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O370" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T370" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U370" s="2"/>
+      <c r="V370" s="2"/>
+      <c r="W370" s="2"/>
+      <c r="X370" s="2"/>
+      <c r="Y370" s="2"/>
+      <c r="Z370" s="2"/>
+      <c r="AA370" s="2"/>
+      <c r="AB370" s="2"/>
+      <c r="AC370" s="2"/>
+      <c r="AD370" s="2"/>
+    </row>
+    <row r="371" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A371" s="5">
+        <v>45874</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E371" s="2"/>
+      <c r="F371" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G371" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H371" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I371" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J371" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L371" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N371" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O371" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T371" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U371" s="2"/>
+      <c r="V371" s="2"/>
+      <c r="W371" s="2"/>
+      <c r="X371" s="2"/>
+      <c r="Y371" s="2"/>
+      <c r="Z371" s="2"/>
+      <c r="AA371" s="2"/>
+      <c r="AB371" s="2"/>
+      <c r="AC371" s="2"/>
+      <c r="AD371" s="2"/>
+    </row>
+    <row r="372" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A372" s="5">
+        <v>45875</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E372" s="2"/>
+      <c r="F372" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G372" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H372" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I372" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J372" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L372" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N372" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O372" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T372" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U372" s="2"/>
+      <c r="V372" s="2"/>
+      <c r="W372" s="2"/>
+      <c r="X372" s="2"/>
+      <c r="Y372" s="2"/>
+      <c r="Z372" s="2"/>
+      <c r="AA372" s="2"/>
+      <c r="AB372" s="2"/>
+      <c r="AC372" s="2"/>
+      <c r="AD372" s="2"/>
+    </row>
+    <row r="373" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A373" s="5">
+        <v>45876</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E373" s="2"/>
+      <c r="F373" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G373" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H373" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I373" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J373" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L373" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N373" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O373" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T373" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U373" s="2"/>
+      <c r="V373" s="2"/>
+      <c r="W373" s="2"/>
+      <c r="X373" s="2"/>
+      <c r="Y373" s="2"/>
+      <c r="Z373" s="2"/>
+      <c r="AA373" s="2"/>
+      <c r="AB373" s="2"/>
+      <c r="AC373" s="2"/>
+      <c r="AD373" s="2"/>
+    </row>
+    <row r="374" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A374" s="5">
+        <v>45877</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E374" s="2"/>
+      <c r="F374" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G374" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H374" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I374" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J374" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L374" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N374" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O374" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T374" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U374" s="2"/>
+      <c r="V374" s="2"/>
+      <c r="W374" s="2"/>
+      <c r="X374" s="2"/>
+      <c r="Y374" s="2"/>
+      <c r="Z374" s="2"/>
+      <c r="AA374" s="2"/>
+      <c r="AB374" s="2"/>
+      <c r="AC374" s="2"/>
+      <c r="AD374" s="2"/>
+    </row>
+    <row r="375" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A375" s="5">
+        <v>45878</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E375" s="2"/>
+      <c r="F375" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G375" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H375" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I375" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J375" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L375" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N375" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O375" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T375" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U375" s="2"/>
+      <c r="V375" s="2"/>
+      <c r="W375" s="2"/>
+      <c r="X375" s="2"/>
+      <c r="Y375" s="2"/>
+      <c r="Z375" s="2"/>
+      <c r="AA375" s="2"/>
+      <c r="AB375" s="2"/>
+      <c r="AC375" s="2"/>
+      <c r="AD375" s="2"/>
+    </row>
+    <row r="376" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A376" s="5">
+        <v>45879</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E376" s="2"/>
+      <c r="F376" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G376" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H376" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I376" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J376" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L376" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N376" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O376" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T376" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U376" s="2"/>
+      <c r="V376" s="2"/>
+      <c r="W376" s="2"/>
+      <c r="X376" s="2"/>
+      <c r="Y376" s="2"/>
+      <c r="Z376" s="2"/>
+      <c r="AA376" s="2"/>
+      <c r="AB376" s="2"/>
+      <c r="AC376" s="2"/>
+      <c r="AD376" s="2"/>
+    </row>
+    <row r="377" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A377" s="5">
+        <v>45880</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E377" s="2"/>
+      <c r="F377" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G377" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H377" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I377" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J377" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L377" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N377" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O377" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T377" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U377" s="2"/>
+      <c r="V377" s="2"/>
+      <c r="W377" s="2"/>
+      <c r="X377" s="2"/>
+      <c r="Y377" s="2"/>
+      <c r="Z377" s="2"/>
+      <c r="AA377" s="2"/>
+      <c r="AB377" s="2"/>
+      <c r="AC377" s="2"/>
+      <c r="AD377" s="2"/>
+    </row>
+    <row r="378" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A378" s="5">
+        <v>45881</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E378" s="2"/>
+      <c r="F378" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G378" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H378" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I378" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J378" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L378" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N378" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O378" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T378" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U378" s="2"/>
+      <c r="V378" s="2"/>
+      <c r="W378" s="2"/>
+      <c r="X378" s="2"/>
+      <c r="Y378" s="2"/>
+      <c r="Z378" s="2"/>
+      <c r="AA378" s="2"/>
+      <c r="AB378" s="2"/>
+      <c r="AC378" s="2"/>
+      <c r="AD378" s="2"/>
+    </row>
+    <row r="379" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A379" s="5">
+        <v>45882</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E379" s="2"/>
+      <c r="F379" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G379" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H379" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I379" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J379" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L379" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N379" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O379" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T379" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U379" s="2"/>
+      <c r="V379" s="2"/>
+      <c r="W379" s="2"/>
+      <c r="X379" s="2"/>
+      <c r="Y379" s="2"/>
+      <c r="Z379" s="2"/>
+      <c r="AA379" s="2"/>
+      <c r="AB379" s="2"/>
+      <c r="AC379" s="2"/>
+      <c r="AD379" s="2"/>
+    </row>
+    <row r="380" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A380" s="5">
+        <v>45883</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E380" s="2"/>
+      <c r="F380" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G380" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H380" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I380" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J380" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L380" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N380" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O380" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T380" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U380" s="2"/>
+      <c r="V380" s="2"/>
+      <c r="W380" s="2"/>
+      <c r="X380" s="2"/>
+      <c r="Y380" s="2"/>
+      <c r="Z380" s="2"/>
+      <c r="AA380" s="2"/>
+      <c r="AB380" s="2"/>
+      <c r="AC380" s="2"/>
+      <c r="AD380" s="2"/>
+    </row>
+    <row r="381" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A381" s="5">
+        <v>45884</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E381" s="2"/>
+      <c r="F381" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G381" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H381" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I381" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J381" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L381" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N381" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O381" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T381" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U381" s="2"/>
+      <c r="V381" s="2"/>
+      <c r="W381" s="2"/>
+      <c r="X381" s="2"/>
+      <c r="Y381" s="2"/>
+      <c r="Z381" s="2"/>
+      <c r="AA381" s="2"/>
+      <c r="AB381" s="2"/>
+      <c r="AC381" s="2"/>
+      <c r="AD381" s="2"/>
+    </row>
+    <row r="382" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A382" s="5">
+        <v>45885</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E382" s="2"/>
+      <c r="F382" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G382" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H382" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I382" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J382" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L382" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N382" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O382" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T382" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U382" s="2"/>
+      <c r="V382" s="2"/>
+      <c r="W382" s="2"/>
+      <c r="X382" s="2"/>
+      <c r="Y382" s="2"/>
+      <c r="Z382" s="2"/>
+      <c r="AA382" s="2"/>
+      <c r="AB382" s="2"/>
+      <c r="AC382" s="2"/>
+      <c r="AD382" s="2"/>
+    </row>
+    <row r="383" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A383" s="5">
+        <v>45886</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E383" s="2"/>
+      <c r="F383" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G383" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H383" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I383" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J383" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L383" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N383" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O383" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T383" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U383" s="2"/>
+      <c r="V383" s="2"/>
+      <c r="W383" s="2"/>
+      <c r="X383" s="2"/>
+      <c r="Y383" s="2"/>
+      <c r="Z383" s="2"/>
+      <c r="AA383" s="2"/>
+      <c r="AB383" s="2"/>
+      <c r="AC383" s="2"/>
+      <c r="AD383" s="2"/>
+    </row>
+    <row r="384" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A384" s="5">
+        <v>45887</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D384" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E384" s="2"/>
+      <c r="F384" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G384" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H384" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I384" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J384" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L384" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N384" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O384" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T384" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U384" s="2"/>
+      <c r="V384" s="2"/>
+      <c r="W384" s="2"/>
+      <c r="X384" s="2"/>
+      <c r="Y384" s="2"/>
+      <c r="Z384" s="2"/>
+      <c r="AA384" s="2"/>
+      <c r="AB384" s="2"/>
+      <c r="AC384" s="2"/>
+      <c r="AD384" s="2"/>
+    </row>
+    <row r="385" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A385" s="5">
+        <v>45888</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D385" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E385" s="2"/>
+      <c r="F385" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G385" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H385" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I385" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J385" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L385" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N385" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O385" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T385" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U385" s="2"/>
+      <c r="V385" s="2"/>
+      <c r="W385" s="2"/>
+      <c r="X385" s="2"/>
+      <c r="Y385" s="2"/>
+      <c r="Z385" s="2"/>
+      <c r="AA385" s="2"/>
+      <c r="AB385" s="2"/>
+      <c r="AC385" s="2"/>
+      <c r="AD385" s="2"/>
+    </row>
+    <row r="386" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A386" s="5">
+        <v>45889</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D386" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E386" s="2"/>
+      <c r="F386" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G386" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H386" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I386" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J386" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L386" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N386" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O386" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T386" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U386" s="2"/>
+      <c r="V386" s="2"/>
+      <c r="W386" s="2"/>
+      <c r="X386" s="2"/>
+      <c r="Y386" s="2"/>
+      <c r="Z386" s="2"/>
+      <c r="AA386" s="2"/>
+      <c r="AB386" s="2"/>
+      <c r="AC386" s="2"/>
+      <c r="AD386" s="2"/>
+    </row>
+    <row r="387" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A387" s="5">
+        <v>45890</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D387" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E387" s="2"/>
+      <c r="F387" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G387" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H387" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I387" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J387" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L387" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N387" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O387" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T387" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U387" s="2"/>
+      <c r="V387" s="2"/>
+      <c r="W387" s="2"/>
+      <c r="X387" s="2"/>
+      <c r="Y387" s="2"/>
+      <c r="Z387" s="2"/>
+      <c r="AA387" s="2"/>
+      <c r="AB387" s="2"/>
+      <c r="AC387" s="2"/>
+      <c r="AD387" s="2"/>
+    </row>
+    <row r="388" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A388" s="5">
+        <v>45891</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D388" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E388" s="2"/>
+      <c r="F388" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G388" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H388" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I388" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J388" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L388" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N388" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O388" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T388" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U388" s="2"/>
+      <c r="V388" s="2"/>
+      <c r="W388" s="2"/>
+      <c r="X388" s="2"/>
+      <c r="Y388" s="2"/>
+      <c r="Z388" s="2"/>
+      <c r="AA388" s="2"/>
+      <c r="AB388" s="2"/>
+      <c r="AC388" s="2"/>
+      <c r="AD388" s="2"/>
+    </row>
+    <row r="389" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A389" s="5">
+        <v>45892</v>
+      </c>
+      <c r="B389" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D389" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E389" s="2"/>
+      <c r="F389" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G389" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H389" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I389" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J389" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L389" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N389" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O389" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T389" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U389" s="2"/>
+      <c r="V389" s="2"/>
+      <c r="W389" s="2"/>
+      <c r="X389" s="2"/>
+      <c r="Y389" s="2"/>
+      <c r="Z389" s="2"/>
+      <c r="AA389" s="2"/>
+      <c r="AB389" s="2"/>
+      <c r="AC389" s="2"/>
+      <c r="AD389" s="2"/>
+    </row>
+    <row r="390" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A390" s="5">
+        <v>45893</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D390" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E390" s="2"/>
+      <c r="F390" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G390" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H390" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I390" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J390" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L390" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N390" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O390" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T390" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U390" s="2"/>
+      <c r="V390" s="2"/>
+      <c r="W390" s="2"/>
+      <c r="X390" s="2"/>
+      <c r="Y390" s="2"/>
+      <c r="Z390" s="2"/>
+      <c r="AA390" s="2"/>
+      <c r="AB390" s="2"/>
+      <c r="AC390" s="2"/>
+      <c r="AD390" s="2"/>
+    </row>
+    <row r="391" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A391" s="5">
+        <v>45894</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E391" s="2"/>
+      <c r="F391" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G391" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H391" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I391" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J391" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L391" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N391" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O391" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T391" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U391" s="2"/>
+      <c r="V391" s="2"/>
+      <c r="W391" s="2"/>
+      <c r="X391" s="2"/>
+      <c r="Y391" s="2"/>
+      <c r="Z391" s="2"/>
+      <c r="AA391" s="2"/>
+      <c r="AB391" s="2"/>
+      <c r="AC391" s="2"/>
+      <c r="AD391" s="2"/>
+    </row>
+    <row r="392" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A392" s="5">
+        <v>45895</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E392" s="2"/>
+      <c r="F392" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G392" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H392" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I392" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J392" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L392" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N392" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O392" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T392" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U392" s="2"/>
+      <c r="V392" s="2"/>
+      <c r="W392" s="2"/>
+      <c r="X392" s="2"/>
+      <c r="Y392" s="2"/>
+      <c r="Z392" s="2"/>
+      <c r="AA392" s="2"/>
+      <c r="AB392" s="2"/>
+      <c r="AC392" s="2"/>
+      <c r="AD392" s="2"/>
+    </row>
+    <row r="393" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A393" s="5">
+        <v>45896</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E393" s="2"/>
+      <c r="F393" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G393" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H393" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I393" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J393" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L393" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N393" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O393" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T393" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U393" s="2"/>
+      <c r="V393" s="2"/>
+      <c r="W393" s="2"/>
+      <c r="X393" s="2"/>
+      <c r="Y393" s="2"/>
+      <c r="Z393" s="2"/>
+      <c r="AA393" s="2"/>
+      <c r="AB393" s="2"/>
+      <c r="AC393" s="2"/>
+      <c r="AD393" s="2"/>
+    </row>
+    <row r="394" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A394" s="5">
+        <v>45897</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D394" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E394" s="2"/>
+      <c r="F394" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G394" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H394" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I394" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J394" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L394" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N394" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O394" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T394" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U394" s="2"/>
+      <c r="V394" s="2"/>
+      <c r="W394" s="2"/>
+      <c r="X394" s="2"/>
+      <c r="Y394" s="2"/>
+      <c r="Z394" s="2"/>
+      <c r="AA394" s="2"/>
+      <c r="AB394" s="2"/>
+      <c r="AC394" s="2"/>
+      <c r="AD394" s="2"/>
+    </row>
+    <row r="395" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A395" s="5">
+        <v>45898</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E395" s="2"/>
+      <c r="F395" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G395" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H395" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I395" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J395" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L395" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N395" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O395" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T395" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U395" s="2"/>
+      <c r="V395" s="2"/>
+      <c r="W395" s="2"/>
+      <c r="X395" s="2"/>
+      <c r="Y395" s="2"/>
+      <c r="Z395" s="2"/>
+      <c r="AA395" s="2"/>
+      <c r="AB395" s="2"/>
+      <c r="AC395" s="2"/>
+      <c r="AD395" s="2"/>
+    </row>
+    <row r="396" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A396" s="5">
+        <v>45899</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E396" s="2"/>
+      <c r="F396" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G396" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H396" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I396" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J396" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L396" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N396" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O396" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T396" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U396" s="2"/>
+      <c r="V396" s="2"/>
+      <c r="W396" s="2"/>
+      <c r="X396" s="2"/>
+      <c r="Y396" s="2"/>
+      <c r="Z396" s="2"/>
+      <c r="AA396" s="2"/>
+      <c r="AB396" s="2"/>
+      <c r="AC396" s="2"/>
+      <c r="AD396" s="2"/>
+    </row>
+    <row r="397" spans="1:30" ht="13" x14ac:dyDescent="0.15">
+      <c r="A397" s="5">
+        <v>45900</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E397" s="2"/>
+      <c r="F397" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G397" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H397" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I397" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J397" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L397" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N397" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O397" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U397" s="2"/>
+      <c r="V397" s="2"/>
+      <c r="W397" s="2"/>
+      <c r="X397" s="2"/>
+      <c r="Y397" s="2"/>
+      <c r="Z397" s="2"/>
+      <c r="AA397" s="2"/>
+      <c r="AB397" s="2"/>
+      <c r="AC397" s="2"/>
+      <c r="AD397" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23391,13 +25563,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S366"/>
+  <dimension ref="A1:S397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B345" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L48" sqref="L48:L56"/>
+      <selection pane="bottomRight" activeCell="A386" sqref="A386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -43987,6 +46159,1773 @@
         <v>24</v>
       </c>
     </row>
+    <row r="367" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A367" s="5">
+        <v>45870</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D367" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E367" s="1"/>
+      <c r="F367" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G367" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H367" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I367" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J367" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M367" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N367" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O367" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R367" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S367" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="368" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A368" s="5">
+        <v>45871</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D368" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E368" s="1"/>
+      <c r="F368" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G368" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H368" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I368" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J368" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M368" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N368" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O368" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S368" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="369" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A369" s="5">
+        <v>45872</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D369" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E369" s="1"/>
+      <c r="F369" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G369" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H369" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I369" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J369" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M369" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N369" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O369" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R369" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S369" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="370" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A370" s="5">
+        <v>45873</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D370" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E370" s="1"/>
+      <c r="F370" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G370" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H370" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I370" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J370" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M370" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N370" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O370" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R370" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S370" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="371" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A371" s="5">
+        <v>45874</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D371" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E371" s="1"/>
+      <c r="F371" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I371" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J371" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M371" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N371" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O371" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R371" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S371" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="372" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A372" s="5">
+        <v>45875</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D372" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E372" s="1"/>
+      <c r="F372" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G372" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H372" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I372" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J372" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M372" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N372" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O372" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R372" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S372" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="373" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A373" s="5">
+        <v>45876</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D373" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E373" s="1"/>
+      <c r="F373" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G373" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H373" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I373" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J373" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M373" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N373" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O373" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R373" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S373" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="374" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A374" s="5">
+        <v>45877</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D374" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E374" s="1"/>
+      <c r="F374" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H374" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I374" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J374" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M374" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N374" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O374" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R374" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S374" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="375" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A375" s="5">
+        <v>45878</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D375" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E375" s="1"/>
+      <c r="F375" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G375" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I375" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J375" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M375" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N375" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O375" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S375" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="376" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A376" s="5">
+        <v>45879</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D376" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E376" s="1"/>
+      <c r="F376" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G376" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H376" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I376" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J376" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M376" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N376" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O376" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R376" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S376" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="377" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A377" s="5">
+        <v>45880</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D377" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E377" s="1"/>
+      <c r="F377" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H377" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I377" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J377" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M377" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N377" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O377" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R377" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S377" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="378" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A378" s="5">
+        <v>45881</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D378" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E378" s="1"/>
+      <c r="F378" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I378" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J378" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M378" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N378" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O378" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R378" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S378" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="379" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A379" s="5">
+        <v>45882</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D379" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E379" s="1"/>
+      <c r="F379" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G379" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H379" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I379" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J379" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M379" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N379" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O379" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R379" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S379" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="380" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A380" s="5">
+        <v>45883</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D380" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E380" s="1"/>
+      <c r="F380" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I380" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J380" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M380" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N380" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O380" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R380" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S380" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="381" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A381" s="5">
+        <v>45884</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D381" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E381" s="1"/>
+      <c r="F381" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G381" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H381" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I381" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J381" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M381" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N381" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O381" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S381" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="382" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A382" s="5">
+        <v>45885</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D382" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E382" s="1"/>
+      <c r="F382" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I382" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J382" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M382" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N382" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O382" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R382" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S382" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="383" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A383" s="5">
+        <v>45886</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D383" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E383" s="1"/>
+      <c r="F383" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G383" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H383" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I383" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J383" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M383" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N383" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O383" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R383" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S383" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="384" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A384" s="5">
+        <v>45887</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D384" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E384" s="1"/>
+      <c r="F384" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G384" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H384" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I384" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J384" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M384" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N384" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O384" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R384" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S384" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="385" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A385" s="5">
+        <v>45888</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D385" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E385" s="1"/>
+      <c r="F385" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G385" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H385" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I385" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J385" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M385" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N385" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O385" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R385" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S385" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="386" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A386" s="5">
+        <v>45889</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D386" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E386" s="1"/>
+      <c r="F386" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H386" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I386" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J386" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M386" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N386" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O386" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S386" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="387" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A387" s="5">
+        <v>45890</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D387" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E387" s="1"/>
+      <c r="F387" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G387" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H387" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I387" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J387" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M387" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N387" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O387" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R387" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S387" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="388" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A388" s="5">
+        <v>45891</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D388" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E388" s="1"/>
+      <c r="F388" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G388" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H388" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I388" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J388" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M388" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N388" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O388" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R388" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S388" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="389" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A389" s="5">
+        <v>45892</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D389" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E389" s="1"/>
+      <c r="F389" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H389" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I389" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J389" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M389" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N389" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O389" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S389" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="390" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A390" s="5">
+        <v>45893</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D390" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E390" s="1"/>
+      <c r="F390" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G390" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H390" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I390" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J390" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M390" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N390" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O390" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R390" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S390" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="391" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A391" s="5">
+        <v>45894</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D391" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E391" s="1"/>
+      <c r="F391" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H391" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I391" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J391" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M391" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N391" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O391" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R391" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S391" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="392" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A392" s="5">
+        <v>45895</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D392" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E392" s="1"/>
+      <c r="F392" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G392" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H392" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I392" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J392" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M392" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N392" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O392" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S392" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="393" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A393" s="5">
+        <v>45896</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D393" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E393" s="1"/>
+      <c r="F393" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H393" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I393" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J393" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M393" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N393" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O393" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S393" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="394" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A394" s="5">
+        <v>45897</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D394" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E394" s="1"/>
+      <c r="F394" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I394" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J394" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M394" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N394" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O394" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R394" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S394" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="395" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A395" s="5">
+        <v>45898</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D395" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E395" s="1"/>
+      <c r="F395" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G395" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H395" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I395" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J395" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M395" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N395" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O395" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R395" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S395" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="396" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A396" s="5">
+        <v>45899</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D396" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E396" s="1"/>
+      <c r="F396" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H396" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I396" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J396" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M396" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N396" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O396" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R396" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S396" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="397" spans="1:19" ht="13" x14ac:dyDescent="0.15">
+      <c r="A397" s="5">
+        <v>45900</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D397" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E397" s="1"/>
+      <c r="F397" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G397" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H397" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I397" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J397" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M397" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N397" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O397" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R397" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S397" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>